<commit_message>
Recurring Deposit 16 Test cases
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/4002-CREATECLIENT-PERSON.xlsx
+++ b/Mifos Automation Excels/Client/4002-CREATECLIENT-PERSON.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mifosx-e2e-testing\Mifos Automation Excels\Client\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="180" yWindow="495" windowWidth="15015" windowHeight="7620"/>
+    <workbookView xWindow="180" yWindow="495" windowWidth="15015" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="9" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>office</t>
   </si>
@@ -106,12 +111,6 @@
   </si>
   <si>
     <t>New Client 1</t>
-  </si>
-  <si>
-    <t>verifyactivationdate</t>
-  </si>
-  <si>
-    <t>Not activated</t>
   </si>
   <si>
     <t>verifymobilenumber</t>
@@ -141,7 +140,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
@@ -225,11 +224,42 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -278,7 +308,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -311,9 +341,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -346,6 +393,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -524,7 +588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
@@ -567,7 +631,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="2"/>
@@ -708,10 +772,10 @@
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="3:6" ht="15" x14ac:dyDescent="0.25">
@@ -728,15 +792,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -752,47 +816,39 @@
       <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>31</v>
+      <c r="B2" s="6">
+        <v>9874563212</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="6">
-        <v>9874563212</v>
+        <v>31</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>26</v>
+        <v>33</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="12">
+        <v>34</v>
+      </c>
+      <c r="B6" s="12">
         <v>32906</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Share Product 15 Test Cases
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/4002-CREATECLIENT-PERSON.xlsx
+++ b/Mifos Automation Excels/Client/4002-CREATECLIENT-PERSON.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -589,7 +589,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -678,8 +678,8 @@
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="6">
-        <v>9874563212</v>
+      <c r="B7">
+        <v>9901020304</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="2"/>
@@ -795,7 +795,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -816,8 +816,8 @@
       <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="6">
-        <v>9874563212</v>
+      <c r="B2">
+        <v>9901020304</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>